<commit_message>
Actualització de les hores
</commit_message>
<xml_diff>
--- a/Registre d'Hores.xlsx
+++ b/Registre d'Hores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pruiz\Desktop\Jo\Educació\Universitat\5é any\1r Quadrimestre\Disseny de Serveis i Aplicacions\Projecte\Projecte-DSA-Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD39D31F-2942-46CD-81DB-676186D71B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B12498-0B62-45BF-998C-B649FBBFAE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{ADC46AAA-F34B-4A94-A1EC-1AAAB9D9DEE2}"/>
   </bookViews>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FECC660B-557D-4A10-B301-873BED8CD41A}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -438,6 +438,14 @@
       </c>
       <c r="C1">
         <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="1">
+        <v>45972</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>